<commit_message>
added graphs to data before 26th xls file
</commit_message>
<xml_diff>
--- a/data-before_26th.xlsx
+++ b/data-before_26th.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="data.csv" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -219,6 +222,758 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(data.csv!$B$25,data.csv!$C$25,data.csv!$D$25,data.csv!$E$25,data.csv!$F$25,data.csv!$G$25,data.csv!$H$25,data.csv!$I$25)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>139.779695290284</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>79.22294495737506</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>136.03891363706</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>106.6558556618187</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>144.2478327414852</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>92.83017330668766</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(data.csv!$B$25,data.csv!$C$25,data.csv!$D$25,data.csv!$E$25,data.csv!$F$25,data.csv!$G$25,data.csv!$H$25,data.csv!$I$25)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>139.779695290284</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>79.22294495737506</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>136.03891363706</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>106.6558556618187</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>144.2478327414852</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>92.83017330668766</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>data.csv!$B$22:$I$22</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>all_ribbon_time</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>all_cmap_time</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>switched_parent_ribbon_time</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>switched_parent_cmap_time</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>same_parent_ribbon_time</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>same_parent_cmap_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data.csv!$B$23:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3214.59967320261</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2776.49673202614</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3430.73799475957</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2899.0725487886</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2255.496405228754</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2532.747773386742</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2099068632"/>
+        <c:axId val="2144128088"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2099068632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2144128088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2144128088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2099068632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(data.csv!$L$25,data.csv!$M$25)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.0719592078129255</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0466348966698415</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(data.csv!$L$25,data.csv!$M$25)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.0719592078129255</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0466348966698415</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>data.csv!$L$22:$M$22</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ribbin_errors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cmap_errors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data.csv!$L$23:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.352941176470588</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.176470588235294</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2140696232"/>
+        <c:axId val="2100267624"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2140696232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2100267624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2100267624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2140696232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(data.csv!$N$25,data.csv!$O$25)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.129526574063266</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0927129537758662</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(data.csv!$N$25,data.csv!$O$25)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.129526574063266</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0927129537758662</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>data.csv!$N$22:$O$22</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ribbon_rating</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cmap_rating</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data.csv!$N$23:$O$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.882352941176471</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2142126904"/>
+        <c:axId val="2099044856"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2142126904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2099044856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2099044856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2142126904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="data.csv"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="58">
+          <cell r="L58" t="str">
+            <v>ribbin_errors</v>
+          </cell>
+          <cell r="M58" t="str">
+            <v>cmap_errors</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="L59">
+            <v>0.81132075471698117</v>
+          </cell>
+          <cell r="M59">
+            <v>0.24528301886792453</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="L61">
+            <v>0.12970631835590588</v>
+          </cell>
+          <cell r="M61">
+            <v>9.8487093977041057E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1725,6 +2480,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
formatted charts for before 26th
</commit_message>
<xml_diff>
--- a/data-before_26th.xlsx
+++ b/data-before_26th.xlsx
@@ -9,9 +9,6 @@
   <sheets>
     <sheet name="data.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -22,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
   <si>
     <t>age</t>
   </si>
@@ -102,37 +99,40 @@
     <t>47 males + 23 females</t>
   </si>
   <si>
-    <t>all_ribbon_time</t>
-  </si>
-  <si>
-    <t>all_cmap_time</t>
-  </si>
-  <si>
-    <t>switched_parent_ribbon_time</t>
-  </si>
-  <si>
-    <t>switched_parent_cmap_time</t>
-  </si>
-  <si>
-    <t>same_parent_ribbon_time</t>
-  </si>
-  <si>
-    <t>same_parent_cmap_time</t>
-  </si>
-  <si>
     <t>Stdev</t>
   </si>
   <si>
     <t>Stderror=stddev/sqrt(samplesize)</t>
   </si>
   <si>
-    <t>ribbin_errors</t>
-  </si>
-  <si>
-    <t>ribbon_rating</t>
-  </si>
-  <si>
-    <t>cmap_rating</t>
+    <t>Ribbon</t>
+  </si>
+  <si>
+    <t>CommandMaps</t>
+  </si>
+  <si>
+    <t>Ribbon (Different Parent)</t>
+  </si>
+  <si>
+    <t>CommandMap (Different Parent)</t>
+  </si>
+  <si>
+    <t>Ribbon (Same Parent)</t>
+  </si>
+  <si>
+    <t>CommandMap (Same Parent)</t>
+  </si>
+  <si>
+    <t>Errors on Ribbon</t>
+  </si>
+  <si>
+    <t>Errors on CommandMaps</t>
+  </si>
+  <si>
+    <t>Rating for Ribbon</t>
+  </si>
+  <si>
+    <t>Rating for CommandMaps</t>
   </si>
 </sst>
 </file>
@@ -238,6 +238,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean Time per Trial</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -386,22 +405,22 @@
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>all_ribbon_time</c:v>
+                  <c:v>Ribbon</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>all_cmap_time</c:v>
+                  <c:v>CommandMaps</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>switched_parent_ribbon_time</c:v>
+                  <c:v>Ribbon (Different Parent)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>switched_parent_cmap_time</c:v>
+                  <c:v>CommandMap (Different Parent)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>same_parent_ribbon_time</c:v>
+                  <c:v>Ribbon (Same Parent)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>same_parent_cmap_time</c:v>
+                  <c:v>CommandMap (Same Parent)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -443,11 +462,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099068632"/>
-        <c:axId val="2144128088"/>
+        <c:axId val="2141131928"/>
+        <c:axId val="2096566200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099068632"/>
+        <c:axId val="2141131928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -456,7 +475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144128088"/>
+        <c:crossAx val="2096566200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -464,7 +483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144128088"/>
+        <c:axId val="2096566200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,7 +494,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099068632"/>
+        <c:crossAx val="2141131928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -511,6 +530,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean Rating</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -583,10 +621,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>ribbin_errors</c:v>
+                  <c:v>Errors on Ribbon</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cmap_errors</c:v>
+                  <c:v>Errors on CommandMaps</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -616,11 +654,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2140696232"/>
-        <c:axId val="2100267624"/>
+        <c:axId val="2096252728"/>
+        <c:axId val="2100146616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140696232"/>
+        <c:axId val="2096252728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100267624"/>
+        <c:crossAx val="2100146616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -637,7 +675,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100267624"/>
+        <c:axId val="2100146616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,7 +686,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140696232"/>
+        <c:crossAx val="2096252728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -684,6 +722,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean Errors after 72 Trial</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Experiment</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -756,10 +818,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>ribbon_rating</c:v>
+                  <c:v>Rating for Ribbon</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cmap_rating</c:v>
+                  <c:v>Rating for CommandMaps</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -789,11 +851,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2142126904"/>
-        <c:axId val="2099044856"/>
+        <c:axId val="2096375848"/>
+        <c:axId val="2096158696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142126904"/>
+        <c:axId val="2096375848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -802,7 +864,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099044856"/>
+        <c:crossAx val="2096158696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -810,7 +872,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099044856"/>
+        <c:axId val="2096158696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,7 +883,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142126904"/>
+        <c:crossAx val="2096375848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -847,16 +909,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -884,9 +946,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -909,14 +971,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -936,44 +998,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="data.csv"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="58">
-          <cell r="L58" t="str">
-            <v>ribbin_errors</v>
-          </cell>
-          <cell r="M58" t="str">
-            <v>cmap_errors</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="L59">
-            <v>0.81132075471698117</v>
-          </cell>
-          <cell r="M59">
-            <v>0.24528301886792453</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="L61">
-            <v>0.12970631835590588</v>
-          </cell>
-          <cell r="M61">
-            <v>9.8487093977041057E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1300,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2304,34 +2328,34 @@
     </row>
     <row r="22" spans="1:17">
       <c r="B22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L22" t="s">
         <v>34</v>
       </c>
       <c r="M22" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="N22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2381,7 +2405,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <f>STDEV(D2:D18)</f>
@@ -2426,7 +2450,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <f>B24/(71 ^ 0.5)</f>

</xml_diff>

<commit_message>
fixed std error on  before 26th map
</commit_message>
<xml_diff>
--- a/data-before_26th.xlsx
+++ b/data-before_26th.xlsx
@@ -339,28 +339,28 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>139.779695290284</c:v>
+                    <c:v>285.6595864163548</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>79.22294495737506</c:v>
+                    <c:v>161.9032982166077</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>136.03891363706</c:v>
+                    <c:v>278.0147697803286</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>106.6558556618187</c:v>
+                    <c:v>217.9663330497711</c:v>
                   </c:pt>
                   <c:pt idx="5">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>144.2478327414852</c:v>
+                    <c:v>294.7908575477657</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>92.83017330668766</c:v>
+                    <c:v>189.7115947969174</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -372,28 +372,28 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>139.779695290284</c:v>
+                    <c:v>285.6595864163548</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>79.22294495737506</c:v>
+                    <c:v>161.9032982166077</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>136.03891363706</c:v>
+                    <c:v>278.0147697803286</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>106.6558556618187</c:v>
+                    <c:v>217.9663330497711</c:v>
                   </c:pt>
                   <c:pt idx="5">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>144.2478327414852</c:v>
+                    <c:v>294.7908575477657</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>92.83017330668766</c:v>
+                    <c:v>189.7115947969174</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -591,10 +591,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.0719592078129255</c:v>
+                    <c:v>0.147058823529412</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0466348966698415</c:v>
+                    <c:v>0.0953050102707038</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -606,10 +606,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.0719592078129255</c:v>
+                    <c:v>0.147058823529412</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0466348966698415</c:v>
+                    <c:v>0.0953050102707038</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -788,10 +788,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.129526574063266</c:v>
+                    <c:v>0.264705882352941</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0927129537758662</c:v>
+                    <c:v>0.189472040098899</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -803,10 +803,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.129526574063266</c:v>
+                    <c:v>0.264705882352941</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0927129537758662</c:v>
+                    <c:v>0.189472040098899</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2453,52 +2453,52 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <f>B24/(71 ^ 0.5)</f>
-        <v>139.77969529028397</v>
+        <f>B24/(17 ^ 0.5)</f>
+        <v>285.65958641635484</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:O25" si="0">C24/(71 ^ 0.5)</f>
-        <v>79.222944957375063</v>
+        <f>C24/(17 ^ 0.5)</f>
+        <v>161.90329821660771</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C25:O25" si="0">D24/(71 ^ 0.5)</f>
         <v>0</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>136.03891363706001</v>
+        <f>E24/(17 ^ 0.5)</f>
+        <v>278.01476978032861</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
-        <v>106.65585566181866</v>
+        <f>F24/(17 ^ 0.5)</f>
+        <v>217.96633304977109</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H25">
-        <f t="shared" si="0"/>
-        <v>144.24783274148521</v>
+        <f>H24/(17 ^ 0.5)</f>
+        <v>294.79085754776565</v>
       </c>
       <c r="I25">
-        <f t="shared" si="0"/>
-        <v>92.830173306687655</v>
+        <f>I24/(17 ^ 0.5)</f>
+        <v>189.71159479691741</v>
       </c>
       <c r="L25">
-        <f t="shared" si="0"/>
-        <v>7.1959207812925474E-2</v>
+        <f>L24/(17 ^ 0.5)</f>
+        <v>0.14705882352941177</v>
       </c>
       <c r="M25">
-        <f t="shared" si="0"/>
-        <v>4.6634896669841497E-2</v>
+        <f>M24/(17 ^ 0.5)</f>
+        <v>9.530501027070383E-2</v>
       </c>
       <c r="N25">
-        <f t="shared" si="0"/>
-        <v>0.12952657406326584</v>
+        <f>N24/(17 ^ 0.5)</f>
+        <v>0.26470588235294118</v>
       </c>
       <c r="O25">
-        <f t="shared" si="0"/>
-        <v>9.2712953775866178E-2</v>
+        <f>O24/(17 ^ 0.5)</f>
+        <v>0.1894720400988989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>